<commit_message>
Added Niederösterreich and Oberösterreich to the Gemeinderatswahlen.
</commit_message>
<xml_diff>
--- a/Gemeinderatswahlen/csv/NÖ_BEREINIGT_FERTIG.xlsx
+++ b/Gemeinderatswahlen/csv/NÖ_BEREINIGT_FERTIG.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkoller/Downloads/Gemeinderatswahlen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkoller/Downloads/geowahl/Gemeinderatswahlen/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1815,12 +1815,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -2101,7 +2100,7 @@
   <dimension ref="A1:F570"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:M570"/>
+      <selection sqref="A1:F570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2139,7 +2138,7 @@
       <c r="C2" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>1154</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -2153,13 +2152,13 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>5310</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>1935</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>2812</v>
       </c>
       <c r="E3" s="1">
@@ -2179,7 +2178,7 @@
       <c r="C4" s="1">
         <v>220</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>1659</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -2199,7 +2198,7 @@
       <c r="C5" s="1">
         <v>191</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>1142</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -2219,7 +2218,7 @@
       <c r="C6" s="1">
         <v>276</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>1189</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -2239,7 +2238,7 @@
       <c r="C7" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>1047</v>
       </c>
       <c r="E7" s="1">
@@ -2253,7 +2252,7 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>1002</v>
       </c>
       <c r="C8" s="1">
@@ -2319,7 +2318,7 @@
       <c r="C11" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <v>1341</v>
       </c>
       <c r="E11" s="1">
@@ -2359,7 +2358,7 @@
       <c r="C13" s="1">
         <v>170</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="1">
         <v>1631</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2379,7 +2378,7 @@
       <c r="C14" s="1">
         <v>271</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
         <v>1553</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -2419,7 +2418,7 @@
       <c r="C16" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <v>1013</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -2439,7 +2438,7 @@
       <c r="C17" s="1">
         <v>307</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="1">
         <v>1120</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2459,7 +2458,7 @@
       <c r="C18" s="1">
         <v>157</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="1">
         <v>1205</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -2539,7 +2538,7 @@
       <c r="C22" s="1">
         <v>246</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="1">
         <v>1043</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2579,7 +2578,7 @@
       <c r="C24" s="1">
         <v>380</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="1">
         <v>2129</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -2593,13 +2592,13 @@
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="1">
         <v>2952</v>
       </c>
       <c r="C25" s="1">
         <v>353</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="1">
         <v>1242</v>
       </c>
       <c r="E25" s="1">
@@ -2619,7 +2618,7 @@
       <c r="C26" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="1">
         <v>1301</v>
       </c>
       <c r="E26" s="1">
@@ -2639,7 +2638,7 @@
       <c r="C27" s="1">
         <v>99</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="1">
         <v>1607</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -2719,7 +2718,7 @@
       <c r="C31" s="1">
         <v>118</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="1">
         <v>1153</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -2779,7 +2778,7 @@
       <c r="C34" s="1">
         <v>124</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="1">
         <v>1545</v>
       </c>
       <c r="E34" s="1">
@@ -2873,16 +2872,16 @@
       <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="1">
         <v>2396</v>
       </c>
       <c r="C39" s="1">
         <v>636</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="1">
         <v>4596</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="1">
         <v>1640</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -2893,7 +2892,7 @@
       <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="1">
         <v>2450</v>
       </c>
       <c r="C40" s="1">
@@ -2913,7 +2912,7 @@
       <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="1">
         <v>2720</v>
       </c>
       <c r="C41" s="1">
@@ -3073,13 +3072,13 @@
       <c r="A49" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="1">
         <v>1508</v>
       </c>
       <c r="C49" s="1">
         <v>480</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="1">
         <v>1255</v>
       </c>
       <c r="E49" s="1">
@@ -3099,7 +3098,7 @@
       <c r="C50" s="1">
         <v>150</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="1">
         <v>2153</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -3139,7 +3138,7 @@
       <c r="C52" s="1">
         <v>199</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="1">
         <v>1102</v>
       </c>
       <c r="E52" s="1">
@@ -3159,7 +3158,7 @@
       <c r="C53" s="1">
         <v>206</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="1">
         <v>1503</v>
       </c>
       <c r="E53" s="1">
@@ -3173,13 +3172,13 @@
       <c r="A54" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="1">
         <v>2031</v>
       </c>
       <c r="C54" s="1">
         <v>354</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="1">
         <v>1034</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -3213,7 +3212,7 @@
       <c r="A56" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="1">
         <v>1003</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -3333,10 +3332,10 @@
       <c r="A62" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="1">
         <v>6716</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="1">
         <v>1290</v>
       </c>
       <c r="D62" s="1">
@@ -3353,7 +3352,7 @@
       <c r="A63" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="1">
         <v>1703</v>
       </c>
       <c r="C63" s="1">
@@ -3473,13 +3472,13 @@
       <c r="A69" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="1">
         <v>2155</v>
       </c>
       <c r="C69" s="1">
         <v>250</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="1">
         <v>1387</v>
       </c>
       <c r="E69" s="1">
@@ -3559,7 +3558,7 @@
       <c r="C73" s="1">
         <v>294</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="1">
         <v>1673</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -3653,7 +3652,7 @@
       <c r="A78" t="s">
         <v>82</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="1">
         <v>1079</v>
       </c>
       <c r="C78" s="1">
@@ -3699,7 +3698,7 @@
       <c r="C80" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="1">
         <v>1123</v>
       </c>
       <c r="E80" s="1" t="s">
@@ -3739,7 +3738,7 @@
       <c r="C82" s="1">
         <v>0</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="1">
         <v>1001</v>
       </c>
       <c r="E82" s="1" t="s">
@@ -3779,7 +3778,7 @@
       <c r="C84" s="1">
         <v>242</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="1">
         <v>1266</v>
       </c>
       <c r="E84" s="1" t="s">
@@ -3853,7 +3852,7 @@
       <c r="A88" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="1">
         <v>1631</v>
       </c>
       <c r="C88" s="1">
@@ -3919,7 +3918,7 @@
       <c r="C91" s="1">
         <v>305</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D91" s="1">
         <v>2261</v>
       </c>
       <c r="E91" s="1">
@@ -3953,7 +3952,7 @@
       <c r="A93" t="s">
         <v>97</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="1">
         <v>1051</v>
       </c>
       <c r="C93" s="1">
@@ -4033,13 +4032,13 @@
       <c r="A97" t="s">
         <v>101</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="1">
         <v>1763</v>
       </c>
       <c r="C97" s="1">
         <v>525</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="1">
         <v>1881</v>
       </c>
       <c r="E97" s="1">
@@ -4073,13 +4072,13 @@
       <c r="A99" t="s">
         <v>103</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="1">
         <v>2469</v>
       </c>
       <c r="C99" s="1">
         <v>661</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="1">
         <v>1998</v>
       </c>
       <c r="E99" s="1">
@@ -4173,7 +4172,7 @@
       <c r="A104" t="s">
         <v>108</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B104" s="1">
         <v>1231</v>
       </c>
       <c r="C104" s="1">
@@ -4253,7 +4252,7 @@
       <c r="A108" t="s">
         <v>112</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="1">
         <v>1052</v>
       </c>
       <c r="C108" s="1">
@@ -4299,7 +4298,7 @@
       <c r="C110" s="1">
         <v>103</v>
       </c>
-      <c r="D110" s="3">
+      <c r="D110" s="1">
         <v>1047</v>
       </c>
       <c r="E110" s="1" t="s">
@@ -4553,7 +4552,7 @@
       <c r="A123" t="s">
         <v>127</v>
       </c>
-      <c r="B123" s="3">
+      <c r="B123" s="1">
         <v>2613</v>
       </c>
       <c r="C123" s="1">
@@ -4659,7 +4658,7 @@
       <c r="C128" s="1">
         <v>326</v>
       </c>
-      <c r="D128" s="3">
+      <c r="D128" s="1">
         <v>1896</v>
       </c>
       <c r="E128" s="1">
@@ -4713,7 +4712,7 @@
       <c r="A131" t="s">
         <v>135</v>
       </c>
-      <c r="B131" s="3">
+      <c r="B131" s="1">
         <v>1139</v>
       </c>
       <c r="C131" s="1" t="s">
@@ -4773,13 +4772,13 @@
       <c r="A134" t="s">
         <v>138</v>
       </c>
-      <c r="B134" s="3">
+      <c r="B134" s="1">
         <v>1694</v>
       </c>
       <c r="C134" s="1">
         <v>158</v>
       </c>
-      <c r="D134" s="3">
+      <c r="D134" s="1">
         <v>1591</v>
       </c>
       <c r="E134" s="1">
@@ -4799,7 +4798,7 @@
       <c r="C135" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D135" s="3">
+      <c r="D135" s="1">
         <v>1212</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -4893,7 +4892,7 @@
       <c r="A140" t="s">
         <v>144</v>
       </c>
-      <c r="B140" s="3">
+      <c r="B140" s="1">
         <v>1340</v>
       </c>
       <c r="C140" s="1">
@@ -4979,7 +4978,7 @@
       <c r="C144" s="1">
         <v>0</v>
       </c>
-      <c r="D144" s="3">
+      <c r="D144" s="1">
         <v>1291</v>
       </c>
       <c r="E144" s="1" t="s">
@@ -5033,13 +5032,13 @@
       <c r="A147" t="s">
         <v>151</v>
       </c>
-      <c r="B147" s="3">
+      <c r="B147" s="1">
         <v>2070</v>
       </c>
       <c r="C147" s="1">
         <v>264</v>
       </c>
-      <c r="D147" s="3">
+      <c r="D147" s="1">
         <v>1198</v>
       </c>
       <c r="E147" s="1">
@@ -5099,7 +5098,7 @@
       <c r="C150" s="1">
         <v>0</v>
       </c>
-      <c r="D150" s="3">
+      <c r="D150" s="1">
         <v>1301</v>
       </c>
       <c r="E150" s="1" t="s">
@@ -5139,7 +5138,7 @@
       <c r="C152" s="1">
         <v>226</v>
       </c>
-      <c r="D152" s="3">
+      <c r="D152" s="1">
         <v>1001</v>
       </c>
       <c r="E152" s="1">
@@ -5199,7 +5198,7 @@
       <c r="C155" s="1">
         <v>0</v>
       </c>
-      <c r="D155" s="3">
+      <c r="D155" s="1">
         <v>1079</v>
       </c>
       <c r="E155" s="1" t="s">
@@ -5219,7 +5218,7 @@
       <c r="C156" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D156" s="3">
+      <c r="D156" s="1">
         <v>1024</v>
       </c>
       <c r="E156" s="1" t="s">
@@ -5293,13 +5292,13 @@
       <c r="A160" t="s">
         <v>164</v>
       </c>
-      <c r="B160" s="3">
+      <c r="B160" s="1">
         <v>1180</v>
       </c>
-      <c r="C160" s="3">
+      <c r="C160" s="1">
         <v>1176</v>
       </c>
-      <c r="D160" s="3">
+      <c r="D160" s="1">
         <v>3962</v>
       </c>
       <c r="E160" s="1">
@@ -5439,7 +5438,7 @@
       <c r="C167" s="1">
         <v>101</v>
       </c>
-      <c r="D167" s="3">
+      <c r="D167" s="1">
         <v>1979</v>
       </c>
       <c r="E167" s="1">
@@ -5519,7 +5518,7 @@
       <c r="C171" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D171" s="3">
+      <c r="D171" s="1">
         <v>1152</v>
       </c>
       <c r="E171" s="1" t="s">
@@ -5539,7 +5538,7 @@
       <c r="C172" s="1">
         <v>206</v>
       </c>
-      <c r="D172" s="3">
+      <c r="D172" s="1">
         <v>1188</v>
       </c>
       <c r="E172" s="1">
@@ -5559,7 +5558,7 @@
       <c r="C173" s="1">
         <v>118</v>
       </c>
-      <c r="D173" s="3">
+      <c r="D173" s="1">
         <v>1081</v>
       </c>
       <c r="E173" s="1" t="s">
@@ -5579,7 +5578,7 @@
       <c r="C174" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D174" s="3">
+      <c r="D174" s="1">
         <v>1484</v>
       </c>
       <c r="E174" s="1" t="s">
@@ -5679,7 +5678,7 @@
       <c r="C179" s="1">
         <v>126</v>
       </c>
-      <c r="D179" s="3">
+      <c r="D179" s="1">
         <v>1543</v>
       </c>
       <c r="E179" s="1" t="s">
@@ -5699,7 +5698,7 @@
       <c r="C180" s="1">
         <v>290</v>
       </c>
-      <c r="D180" s="3">
+      <c r="D180" s="1">
         <v>1538</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -5739,7 +5738,7 @@
       <c r="C182" s="1">
         <v>438</v>
       </c>
-      <c r="D182" s="3">
+      <c r="D182" s="1">
         <v>2563</v>
       </c>
       <c r="E182" s="1">
@@ -5919,7 +5918,7 @@
       <c r="C191" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D191" s="3">
+      <c r="D191" s="1">
         <v>1087</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -5959,7 +5958,7 @@
       <c r="C193" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D193" s="3">
+      <c r="D193" s="1">
         <v>1099</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -5999,7 +5998,7 @@
       <c r="C195" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D195" s="3">
+      <c r="D195" s="1">
         <v>1851</v>
       </c>
       <c r="E195" s="1">
@@ -6039,7 +6038,7 @@
       <c r="C197" s="1">
         <v>273</v>
       </c>
-      <c r="D197" s="3">
+      <c r="D197" s="1">
         <v>1486</v>
       </c>
       <c r="E197" s="1">
@@ -6079,7 +6078,7 @@
       <c r="C199" s="1">
         <v>174</v>
       </c>
-      <c r="D199" s="3">
+      <c r="D199" s="1">
         <v>1084</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6119,7 +6118,7 @@
       <c r="C201" s="1">
         <v>472</v>
       </c>
-      <c r="D201" s="3">
+      <c r="D201" s="1">
         <v>1310</v>
       </c>
       <c r="E201" s="1">
@@ -6139,7 +6138,7 @@
       <c r="C202" s="1">
         <v>162</v>
       </c>
-      <c r="D202" s="3">
+      <c r="D202" s="1">
         <v>1404</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -6153,13 +6152,13 @@
       <c r="A203" t="s">
         <v>207</v>
       </c>
-      <c r="B203" s="3">
+      <c r="B203" s="1">
         <v>1610</v>
       </c>
       <c r="C203" s="1">
         <v>365</v>
       </c>
-      <c r="D203" s="3">
+      <c r="D203" s="1">
         <v>3687</v>
       </c>
       <c r="E203" s="1">
@@ -6179,7 +6178,7 @@
       <c r="C204" s="1">
         <v>344</v>
       </c>
-      <c r="D204" s="3">
+      <c r="D204" s="1">
         <v>2647</v>
       </c>
       <c r="E204" s="1">
@@ -6219,7 +6218,7 @@
       <c r="C206" s="1">
         <v>200</v>
       </c>
-      <c r="D206" s="3">
+      <c r="D206" s="1">
         <v>1947</v>
       </c>
       <c r="E206" s="1">
@@ -6259,7 +6258,7 @@
       <c r="C208" s="1">
         <v>283</v>
       </c>
-      <c r="D208" s="3">
+      <c r="D208" s="1">
         <v>1437</v>
       </c>
       <c r="E208" s="1">
@@ -6333,13 +6332,13 @@
       <c r="A212" t="s">
         <v>216</v>
       </c>
-      <c r="B212" s="3">
+      <c r="B212" s="1">
         <v>3591</v>
       </c>
-      <c r="C212" s="3">
+      <c r="C212" s="1">
         <v>1040</v>
       </c>
-      <c r="D212" s="3">
+      <c r="D212" s="1">
         <v>2503</v>
       </c>
       <c r="E212" s="1">
@@ -6459,7 +6458,7 @@
       <c r="C218" s="1">
         <v>164</v>
       </c>
-      <c r="D218" s="3">
+      <c r="D218" s="1">
         <v>1505</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -6479,7 +6478,7 @@
       <c r="C219" s="1">
         <v>95</v>
       </c>
-      <c r="D219" s="3">
+      <c r="D219" s="1">
         <v>1057</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -6519,7 +6518,7 @@
       <c r="C221" s="1">
         <v>245</v>
       </c>
-      <c r="D221" s="3">
+      <c r="D221" s="1">
         <v>1501</v>
       </c>
       <c r="E221" s="1">
@@ -6599,7 +6598,7 @@
       <c r="C225" s="1">
         <v>558</v>
       </c>
-      <c r="D225" s="3">
+      <c r="D225" s="1">
         <v>2882</v>
       </c>
       <c r="E225" s="1">
@@ -6639,7 +6638,7 @@
       <c r="C227" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D227" s="3">
+      <c r="D227" s="1">
         <v>1199</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -6679,7 +6678,7 @@
       <c r="C229" s="1">
         <v>170</v>
       </c>
-      <c r="D229" s="3">
+      <c r="D229" s="1">
         <v>1317</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -7013,7 +7012,7 @@
       <c r="A246" t="s">
         <v>250</v>
       </c>
-      <c r="B246" s="3">
+      <c r="B246" s="1">
         <v>1453</v>
       </c>
       <c r="C246" s="1">
@@ -7099,7 +7098,7 @@
       <c r="C250" s="1">
         <v>112</v>
       </c>
-      <c r="D250" s="3">
+      <c r="D250" s="1">
         <v>1180</v>
       </c>
       <c r="E250" s="1" t="s">
@@ -7193,7 +7192,7 @@
       <c r="A255" t="s">
         <v>259</v>
       </c>
-      <c r="B255" s="3">
+      <c r="B255" s="1">
         <v>1810</v>
       </c>
       <c r="C255" s="1">
@@ -7213,7 +7212,7 @@
       <c r="A256" t="s">
         <v>260</v>
       </c>
-      <c r="B256" s="3">
+      <c r="B256" s="1">
         <v>1177</v>
       </c>
       <c r="C256" s="1">
@@ -7359,7 +7358,7 @@
       <c r="C263" s="1">
         <v>204</v>
       </c>
-      <c r="D263" s="3">
+      <c r="D263" s="1">
         <v>1070</v>
       </c>
       <c r="E263" s="1">
@@ -7439,7 +7438,7 @@
       <c r="C267" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D267" s="3">
+      <c r="D267" s="1">
         <v>1063</v>
       </c>
       <c r="E267" s="1" t="s">
@@ -7459,7 +7458,7 @@
       <c r="C268" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D268" s="3">
+      <c r="D268" s="1">
         <v>1256</v>
       </c>
       <c r="E268" s="1" t="s">
@@ -7553,7 +7552,7 @@
       <c r="A273" t="s">
         <v>277</v>
       </c>
-      <c r="B273" s="3">
+      <c r="B273" s="1">
         <v>1672</v>
       </c>
       <c r="C273" s="1">
@@ -7579,7 +7578,7 @@
       <c r="C274" s="1">
         <v>191</v>
       </c>
-      <c r="D274" s="3">
+      <c r="D274" s="1">
         <v>1485</v>
       </c>
       <c r="E274" s="1" t="s">
@@ -7639,7 +7638,7 @@
       <c r="C277" s="1">
         <v>235</v>
       </c>
-      <c r="D277" s="3">
+      <c r="D277" s="1">
         <v>1756</v>
       </c>
       <c r="E277" s="1">
@@ -7659,7 +7658,7 @@
       <c r="C278" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D278" s="3">
+      <c r="D278" s="1">
         <v>1158</v>
       </c>
       <c r="E278" s="1" t="s">
@@ -7713,7 +7712,7 @@
       <c r="A281" t="s">
         <v>285</v>
       </c>
-      <c r="B281" s="3">
+      <c r="B281" s="1">
         <v>1040</v>
       </c>
       <c r="C281" s="1" t="s">
@@ -7759,7 +7758,7 @@
       <c r="C283" s="1">
         <v>544</v>
       </c>
-      <c r="D283" s="3">
+      <c r="D283" s="1">
         <v>1068</v>
       </c>
       <c r="E283" s="1">
@@ -7779,7 +7778,7 @@
       <c r="C284" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D284" s="3">
+      <c r="D284" s="1">
         <v>1348</v>
       </c>
       <c r="E284" s="1" t="s">
@@ -7819,7 +7818,7 @@
       <c r="C286" s="1">
         <v>283</v>
       </c>
-      <c r="D286" s="3">
+      <c r="D286" s="1">
         <v>1112</v>
       </c>
       <c r="E286" s="1" t="s">
@@ -7839,7 +7838,7 @@
       <c r="C287" s="1">
         <v>364</v>
       </c>
-      <c r="D287" s="3">
+      <c r="D287" s="1">
         <v>1264</v>
       </c>
       <c r="E287" s="1" t="s">
@@ -7953,13 +7952,13 @@
       <c r="A293" t="s">
         <v>297</v>
       </c>
-      <c r="B293" s="3">
+      <c r="B293" s="1">
         <v>1700</v>
       </c>
       <c r="C293" s="1">
         <v>282</v>
       </c>
-      <c r="D293" s="3">
+      <c r="D293" s="1">
         <v>1063</v>
       </c>
       <c r="E293" s="1">
@@ -8019,7 +8018,7 @@
       <c r="C296" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D296" s="3">
+      <c r="D296" s="1">
         <v>1076</v>
       </c>
       <c r="E296" s="1" t="s">
@@ -8219,7 +8218,7 @@
       <c r="C306" s="1">
         <v>218</v>
       </c>
-      <c r="D306" s="3">
+      <c r="D306" s="1">
         <v>1463</v>
       </c>
       <c r="E306" s="1">
@@ -8259,7 +8258,7 @@
       <c r="C308" s="1">
         <v>159</v>
       </c>
-      <c r="D308" s="3">
+      <c r="D308" s="1">
         <v>1114</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8439,7 +8438,7 @@
       <c r="C317" s="1">
         <v>329</v>
       </c>
-      <c r="D317" s="3">
+      <c r="D317" s="1">
         <v>2977</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -8473,13 +8472,13 @@
       <c r="A319" t="s">
         <v>323</v>
       </c>
-      <c r="B319" s="3">
+      <c r="B319" s="1">
         <v>1359</v>
       </c>
       <c r="C319" s="1">
         <v>478</v>
       </c>
-      <c r="D319" s="3">
+      <c r="D319" s="1">
         <v>3238</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -8559,7 +8558,7 @@
       <c r="C323" s="1">
         <v>313</v>
       </c>
-      <c r="D323" s="3">
+      <c r="D323" s="1">
         <v>2976</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -8739,7 +8738,7 @@
       <c r="C332" s="1">
         <v>251</v>
       </c>
-      <c r="D332" s="3">
+      <c r="D332" s="1">
         <v>2098</v>
       </c>
       <c r="E332" s="1">
@@ -8819,10 +8818,10 @@
       <c r="C336" s="1">
         <v>215</v>
       </c>
-      <c r="D336" s="3">
+      <c r="D336" s="1">
         <v>1295</v>
       </c>
-      <c r="E336" s="3">
+      <c r="E336" s="1">
         <v>1084</v>
       </c>
       <c r="F336" s="1" t="s">
@@ -8833,13 +8832,13 @@
       <c r="A337" t="s">
         <v>341</v>
       </c>
-      <c r="B337" s="3">
+      <c r="B337" s="1">
         <v>2599</v>
       </c>
       <c r="C337" s="1">
         <v>658</v>
       </c>
-      <c r="D337" s="3">
+      <c r="D337" s="1">
         <v>1371</v>
       </c>
       <c r="E337" s="1">
@@ -8899,7 +8898,7 @@
       <c r="C340" s="1">
         <v>121</v>
       </c>
-      <c r="D340" s="3">
+      <c r="D340" s="1">
         <v>1058</v>
       </c>
       <c r="E340" s="1">
@@ -8913,13 +8912,13 @@
       <c r="A341" t="s">
         <v>345</v>
       </c>
-      <c r="B341" s="3">
+      <c r="B341" s="1">
         <v>2086</v>
       </c>
       <c r="C341" s="1">
         <v>870</v>
       </c>
-      <c r="D341" s="3">
+      <c r="D341" s="1">
         <v>1338</v>
       </c>
       <c r="E341" s="1">
@@ -8959,7 +8958,7 @@
       <c r="C343" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D343" s="3">
+      <c r="D343" s="1">
         <v>1158</v>
       </c>
       <c r="E343" s="1">
@@ -9019,7 +9018,7 @@
       <c r="C346" s="1">
         <v>90</v>
       </c>
-      <c r="D346" s="3">
+      <c r="D346" s="1">
         <v>1147</v>
       </c>
       <c r="E346" s="1">
@@ -9039,7 +9038,7 @@
       <c r="C347" s="1">
         <v>222</v>
       </c>
-      <c r="D347" s="3">
+      <c r="D347" s="1">
         <v>1816</v>
       </c>
       <c r="E347" s="1">
@@ -9053,16 +9052,16 @@
       <c r="A348" t="s">
         <v>352</v>
       </c>
-      <c r="B348" s="3">
+      <c r="B348" s="1">
         <v>1860</v>
       </c>
       <c r="C348" s="1">
         <v>886</v>
       </c>
-      <c r="D348" s="3">
+      <c r="D348" s="1">
         <v>3741</v>
       </c>
-      <c r="E348" s="3">
+      <c r="E348" s="1">
         <v>2189</v>
       </c>
       <c r="F348" s="1">
@@ -9099,7 +9098,7 @@
       <c r="C350" s="1">
         <v>563</v>
       </c>
-      <c r="D350" s="3">
+      <c r="D350" s="1">
         <v>4900</v>
       </c>
       <c r="E350" s="1">
@@ -9113,7 +9112,7 @@
       <c r="A351" t="s">
         <v>355</v>
       </c>
-      <c r="B351" s="3">
+      <c r="B351" s="1">
         <v>1347</v>
       </c>
       <c r="C351" s="1">
@@ -9133,13 +9132,13 @@
       <c r="A352" t="s">
         <v>356</v>
       </c>
-      <c r="B352" s="3">
+      <c r="B352" s="1">
         <v>2287</v>
       </c>
       <c r="C352" s="1">
         <v>434</v>
       </c>
-      <c r="D352" s="3">
+      <c r="D352" s="1">
         <v>1803</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9199,7 +9198,7 @@
       <c r="C355" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D355" s="3">
+      <c r="D355" s="1">
         <v>1038</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9219,7 +9218,7 @@
       <c r="C356" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D356" s="3">
+      <c r="D356" s="1">
         <v>1037</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9353,7 +9352,7 @@
       <c r="A363" t="s">
         <v>367</v>
       </c>
-      <c r="B363" s="3">
+      <c r="B363" s="1">
         <v>1039</v>
       </c>
       <c r="C363" s="1">
@@ -9373,7 +9372,7 @@
       <c r="A364" t="s">
         <v>368</v>
       </c>
-      <c r="B364" s="3">
+      <c r="B364" s="1">
         <v>1026</v>
       </c>
       <c r="C364" s="1">
@@ -9439,7 +9438,7 @@
       <c r="C367" s="1">
         <v>226</v>
       </c>
-      <c r="D367" s="3">
+      <c r="D367" s="1">
         <v>1193</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9493,13 +9492,13 @@
       <c r="A370" t="s">
         <v>374</v>
       </c>
-      <c r="B370" s="3">
+      <c r="B370" s="1">
         <v>2076</v>
       </c>
       <c r="C370" s="1">
         <v>492</v>
       </c>
-      <c r="D370" s="3">
+      <c r="D370" s="1">
         <v>2367</v>
       </c>
       <c r="E370" s="1">
@@ -9539,7 +9538,7 @@
       <c r="C372" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D372" s="3">
+      <c r="D372" s="1">
         <v>1156</v>
       </c>
       <c r="E372" s="1">
@@ -9593,7 +9592,7 @@
       <c r="A375" t="s">
         <v>379</v>
       </c>
-      <c r="B375" s="3">
+      <c r="B375" s="1">
         <v>1171</v>
       </c>
       <c r="C375" s="1">
@@ -9639,7 +9638,7 @@
       <c r="C377" s="1">
         <v>173</v>
       </c>
-      <c r="D377" s="3">
+      <c r="D377" s="1">
         <v>1165</v>
       </c>
       <c r="E377" s="1">
@@ -9833,7 +9832,7 @@
       <c r="A387" t="s">
         <v>391</v>
       </c>
-      <c r="B387" s="3">
+      <c r="B387" s="1">
         <v>5054</v>
       </c>
       <c r="C387" s="1">
@@ -9939,7 +9938,7 @@
       <c r="C392" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D392" s="3">
+      <c r="D392" s="1">
         <v>1036</v>
       </c>
       <c r="E392" s="1" t="s">
@@ -10093,13 +10092,13 @@
       <c r="A400" t="s">
         <v>404</v>
       </c>
-      <c r="B400" s="3">
+      <c r="B400" s="1">
         <v>1235</v>
       </c>
       <c r="C400" s="1">
         <v>255</v>
       </c>
-      <c r="D400" s="3">
+      <c r="D400" s="1">
         <v>1199</v>
       </c>
       <c r="E400" s="1">
@@ -10139,7 +10138,7 @@
       <c r="C402" s="1">
         <v>186</v>
       </c>
-      <c r="D402" s="3">
+      <c r="D402" s="1">
         <v>1034</v>
       </c>
       <c r="E402" s="1">
@@ -10159,7 +10158,7 @@
       <c r="C403" s="1">
         <v>133</v>
       </c>
-      <c r="D403" s="3">
+      <c r="D403" s="1">
         <v>1049</v>
       </c>
       <c r="E403" s="1" t="s">
@@ -10199,7 +10198,7 @@
       <c r="C405" s="1">
         <v>204</v>
       </c>
-      <c r="D405" s="3">
+      <c r="D405" s="1">
         <v>1095</v>
       </c>
       <c r="E405" s="1" t="s">
@@ -10253,13 +10252,13 @@
       <c r="A408" t="s">
         <v>412</v>
       </c>
-      <c r="B408" s="3">
+      <c r="B408" s="1">
         <v>2163</v>
       </c>
       <c r="C408" s="1">
         <v>884</v>
       </c>
-      <c r="D408" s="3">
+      <c r="D408" s="1">
         <v>1068</v>
       </c>
       <c r="E408" s="1">
@@ -10359,7 +10358,7 @@
       <c r="C413" s="1">
         <v>290</v>
       </c>
-      <c r="D413" s="3">
+      <c r="D413" s="1">
         <v>1393</v>
       </c>
       <c r="E413" s="1" t="s">
@@ -10419,7 +10418,7 @@
       <c r="C416" s="1">
         <v>221</v>
       </c>
-      <c r="D416" s="3">
+      <c r="D416" s="1">
         <v>1291</v>
       </c>
       <c r="E416" s="1">
@@ -10499,7 +10498,7 @@
       <c r="C420" s="1">
         <v>350</v>
       </c>
-      <c r="D420" s="3">
+      <c r="D420" s="1">
         <v>2186</v>
       </c>
       <c r="E420" s="1">
@@ -10553,7 +10552,7 @@
       <c r="A423" t="s">
         <v>427</v>
       </c>
-      <c r="B423" s="3">
+      <c r="B423" s="1">
         <v>1774</v>
       </c>
       <c r="C423" s="1">
@@ -10619,7 +10618,7 @@
       <c r="C426" s="1">
         <v>120</v>
       </c>
-      <c r="D426" s="3">
+      <c r="D426" s="1">
         <v>1199</v>
       </c>
       <c r="E426" s="1" t="s">
@@ -10639,7 +10638,7 @@
       <c r="C427" s="1">
         <v>104</v>
       </c>
-      <c r="D427" s="3">
+      <c r="D427" s="1">
         <v>1189</v>
       </c>
       <c r="E427" s="1" t="s">
@@ -10733,13 +10732,13 @@
       <c r="A432" t="s">
         <v>436</v>
       </c>
-      <c r="B432" s="3">
+      <c r="B432" s="1">
         <v>2080</v>
       </c>
       <c r="C432" s="1">
         <v>242</v>
       </c>
-      <c r="D432" s="3">
+      <c r="D432" s="1">
         <v>1276</v>
       </c>
       <c r="E432" s="1">
@@ -10793,7 +10792,7 @@
       <c r="A435" t="s">
         <v>439</v>
       </c>
-      <c r="B435" s="3">
+      <c r="B435" s="1">
         <v>1836</v>
       </c>
       <c r="C435" s="1">
@@ -10813,7 +10812,7 @@
       <c r="A436" t="s">
         <v>440</v>
       </c>
-      <c r="B436" s="3">
+      <c r="B436" s="1">
         <v>1013</v>
       </c>
       <c r="C436" s="1">
@@ -10833,7 +10832,7 @@
       <c r="A437" t="s">
         <v>441</v>
       </c>
-      <c r="B437" s="3">
+      <c r="B437" s="1">
         <v>1121</v>
       </c>
       <c r="C437" s="1">
@@ -10939,7 +10938,7 @@
       <c r="C442" s="1">
         <v>188</v>
       </c>
-      <c r="D442" s="3">
+      <c r="D442" s="1">
         <v>1346</v>
       </c>
       <c r="E442" s="1" t="s">
@@ -10979,7 +10978,7 @@
       <c r="C444" s="1">
         <v>251</v>
       </c>
-      <c r="D444" s="3">
+      <c r="D444" s="1">
         <v>1991</v>
       </c>
       <c r="E444" s="1">
@@ -10999,7 +10998,7 @@
       <c r="C445" s="1">
         <v>92</v>
       </c>
-      <c r="D445" s="3">
+      <c r="D445" s="1">
         <v>1039</v>
       </c>
       <c r="E445" s="1" t="s">
@@ -11079,7 +11078,7 @@
       <c r="C449" s="1">
         <v>0</v>
       </c>
-      <c r="D449" s="3">
+      <c r="D449" s="1">
         <v>1774</v>
       </c>
       <c r="E449" s="1">
@@ -11099,7 +11098,7 @@
       <c r="C450" s="1">
         <v>110</v>
       </c>
-      <c r="D450" s="3">
+      <c r="D450" s="1">
         <v>1113</v>
       </c>
       <c r="E450" s="1" t="s">
@@ -11133,7 +11132,7 @@
       <c r="A452" t="s">
         <v>456</v>
       </c>
-      <c r="B452" s="3">
+      <c r="B452" s="1">
         <v>1393</v>
       </c>
       <c r="C452" s="1">
@@ -11159,7 +11158,7 @@
       <c r="C453" s="1">
         <v>231</v>
       </c>
-      <c r="D453" s="3">
+      <c r="D453" s="1">
         <v>1483</v>
       </c>
       <c r="E453" s="1" t="s">
@@ -11219,7 +11218,7 @@
       <c r="C456" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D456" s="3">
+      <c r="D456" s="1">
         <v>1386</v>
       </c>
       <c r="E456" s="1" t="s">
@@ -11259,7 +11258,7 @@
       <c r="C458" s="1">
         <v>0</v>
       </c>
-      <c r="D458" s="3">
+      <c r="D458" s="1">
         <v>1409</v>
       </c>
       <c r="E458" s="1" t="s">
@@ -11299,7 +11298,7 @@
       <c r="C460" s="1">
         <v>485</v>
       </c>
-      <c r="D460" s="3">
+      <c r="D460" s="1">
         <v>1124</v>
       </c>
       <c r="E460" s="1" t="s">
@@ -11339,7 +11338,7 @@
       <c r="C462" s="1">
         <v>287</v>
       </c>
-      <c r="D462" s="3">
+      <c r="D462" s="1">
         <v>1479</v>
       </c>
       <c r="E462" s="1" t="s">
@@ -11399,7 +11398,7 @@
       <c r="C465" s="1">
         <v>192</v>
       </c>
-      <c r="D465" s="3">
+      <c r="D465" s="1">
         <v>1049</v>
       </c>
       <c r="E465" s="1" t="s">
@@ -11419,7 +11418,7 @@
       <c r="C466" s="1">
         <v>193</v>
       </c>
-      <c r="D466" s="3">
+      <c r="D466" s="1">
         <v>1235</v>
       </c>
       <c r="E466" s="1" t="s">
@@ -11433,13 +11432,13 @@
       <c r="A467" t="s">
         <v>471</v>
       </c>
-      <c r="B467" s="3">
+      <c r="B467" s="1">
         <v>1048</v>
       </c>
       <c r="C467" s="1">
         <v>590</v>
       </c>
-      <c r="D467" s="3">
+      <c r="D467" s="1">
         <v>2361</v>
       </c>
       <c r="E467" s="1">
@@ -11459,7 +11458,7 @@
       <c r="C468" s="1">
         <v>118</v>
       </c>
-      <c r="D468" s="3">
+      <c r="D468" s="1">
         <v>1000</v>
       </c>
       <c r="E468" s="1" t="s">
@@ -11479,7 +11478,7 @@
       <c r="C469" s="1">
         <v>135</v>
       </c>
-      <c r="D469" s="3">
+      <c r="D469" s="1">
         <v>1288</v>
       </c>
       <c r="E469" s="1" t="s">
@@ -11493,13 +11492,13 @@
       <c r="A470" t="s">
         <v>474</v>
       </c>
-      <c r="B470" s="3">
+      <c r="B470" s="1">
         <v>1405</v>
       </c>
       <c r="C470" s="1">
         <v>539</v>
       </c>
-      <c r="D470" s="3">
+      <c r="D470" s="1">
         <v>3988</v>
       </c>
       <c r="E470" s="1">
@@ -11553,7 +11552,7 @@
       <c r="A473" t="s">
         <v>477</v>
       </c>
-      <c r="B473" s="3">
+      <c r="B473" s="1">
         <v>1392</v>
       </c>
       <c r="C473" s="1">
@@ -11573,13 +11572,13 @@
       <c r="A474" t="s">
         <v>478</v>
       </c>
-      <c r="B474" s="3">
+      <c r="B474" s="1">
         <v>2031</v>
       </c>
       <c r="C474" s="1">
         <v>524</v>
       </c>
-      <c r="D474" s="3">
+      <c r="D474" s="1">
         <v>1189</v>
       </c>
       <c r="E474" s="1">
@@ -11779,7 +11778,7 @@
       <c r="C484" s="1">
         <v>266</v>
       </c>
-      <c r="D484" s="3">
+      <c r="D484" s="1">
         <v>1411</v>
       </c>
       <c r="E484" s="1" t="s">
@@ -11819,7 +11818,7 @@
       <c r="C486" s="1">
         <v>157</v>
       </c>
-      <c r="D486" s="3">
+      <c r="D486" s="1">
         <v>1326</v>
       </c>
       <c r="E486" s="1" t="s">
@@ -11839,7 +11838,7 @@
       <c r="C487" s="1">
         <v>842</v>
       </c>
-      <c r="D487" s="3">
+      <c r="D487" s="1">
         <v>1690</v>
       </c>
       <c r="E487" s="1">
@@ -11919,7 +11918,7 @@
       <c r="C491" s="1">
         <v>99</v>
       </c>
-      <c r="D491" s="3">
+      <c r="D491" s="1">
         <v>1228</v>
       </c>
       <c r="E491" s="1" t="s">
@@ -11953,7 +11952,7 @@
       <c r="A493" t="s">
         <v>497</v>
       </c>
-      <c r="B493" s="3">
+      <c r="B493" s="1">
         <v>1460</v>
       </c>
       <c r="C493" s="1">
@@ -11973,7 +11972,7 @@
       <c r="A494" t="s">
         <v>498</v>
       </c>
-      <c r="B494" s="3">
+      <c r="B494" s="1">
         <v>1891</v>
       </c>
       <c r="C494" s="1">
@@ -11999,7 +11998,7 @@
       <c r="C495" s="1">
         <v>143</v>
       </c>
-      <c r="D495" s="3">
+      <c r="D495" s="1">
         <v>1526</v>
       </c>
       <c r="E495" s="1" t="s">
@@ -12013,7 +12012,7 @@
       <c r="A496" t="s">
         <v>500</v>
       </c>
-      <c r="B496" s="3">
+      <c r="B496" s="1">
         <v>1259</v>
       </c>
       <c r="C496" s="1">
@@ -12059,7 +12058,7 @@
       <c r="C498" s="1">
         <v>145</v>
       </c>
-      <c r="D498" s="3">
+      <c r="D498" s="1">
         <v>1021</v>
       </c>
       <c r="E498" s="1" t="s">
@@ -12085,6 +12084,7 @@
       <c r="E499" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F499" s="3"/>
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
@@ -12102,6 +12102,7 @@
       <c r="E500" s="1">
         <v>110</v>
       </c>
+      <c r="F500" s="3"/>
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
@@ -12119,6 +12120,7 @@
       <c r="E501" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F501" s="3"/>
     </row>
     <row r="502" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
@@ -12130,12 +12132,13 @@
       <c r="C502" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D502" s="3">
+      <c r="D502" s="1">
         <v>1267</v>
       </c>
       <c r="E502" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F502" s="3"/>
     </row>
     <row r="503" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
@@ -12147,12 +12150,13 @@
       <c r="C503" s="1">
         <v>215</v>
       </c>
-      <c r="D503" s="3">
+      <c r="D503" s="1">
         <v>1477</v>
       </c>
       <c r="E503" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F503" s="3"/>
     </row>
     <row r="504" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
@@ -12164,12 +12168,13 @@
       <c r="C504" s="1">
         <v>205</v>
       </c>
-      <c r="D504" s="3">
+      <c r="D504" s="1">
         <v>1267</v>
       </c>
       <c r="E504" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F504" s="3"/>
     </row>
     <row r="505" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
@@ -12181,12 +12186,13 @@
       <c r="C505" s="1">
         <v>249</v>
       </c>
-      <c r="D505" s="3">
+      <c r="D505" s="1">
         <v>1451</v>
       </c>
       <c r="E505" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F505" s="3"/>
     </row>
     <row r="506" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
@@ -12204,12 +12210,13 @@
       <c r="E506" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F506" s="3"/>
     </row>
     <row r="507" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
         <v>511</v>
       </c>
-      <c r="B507" s="3">
+      <c r="B507" s="1">
         <v>1012</v>
       </c>
       <c r="C507" s="1">
@@ -12221,6 +12228,7 @@
       <c r="E507" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F507" s="3"/>
     </row>
     <row r="508" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
@@ -12232,12 +12240,13 @@
       <c r="C508" s="1">
         <v>177</v>
       </c>
-      <c r="D508" s="3">
+      <c r="D508" s="1">
         <v>1267</v>
       </c>
       <c r="E508" s="1">
         <v>136</v>
       </c>
+      <c r="F508" s="3"/>
     </row>
     <row r="509" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
@@ -12249,12 +12258,13 @@
       <c r="C509" s="1">
         <v>92</v>
       </c>
-      <c r="D509" s="3">
+      <c r="D509" s="1">
         <v>1067</v>
       </c>
       <c r="E509" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F509" s="3"/>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
@@ -12272,6 +12282,7 @@
       <c r="E510" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F510" s="3"/>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
@@ -12289,6 +12300,7 @@
       <c r="E511" s="1" t="s">
         <v>575</v>
       </c>
+      <c r="F511" s="3"/>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
@@ -12306,8 +12318,9 @@
       <c r="E512" s="1">
         <v>93</v>
       </c>
-    </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F512" s="3"/>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>517</v>
       </c>
@@ -12323,8 +12336,9 @@
       <c r="E513" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F513" s="3"/>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
         <v>518</v>
       </c>
@@ -12340,8 +12354,9 @@
       <c r="E514" s="1">
         <v>68</v>
       </c>
-    </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F514" s="3"/>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>519</v>
       </c>
@@ -12357,12 +12372,13 @@
       <c r="E515" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F515" s="3"/>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
         <v>520</v>
       </c>
-      <c r="B516" s="3">
+      <c r="B516" s="1">
         <v>1507</v>
       </c>
       <c r="C516" s="1">
@@ -12374,12 +12390,13 @@
       <c r="E516" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F516" s="3"/>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>521</v>
       </c>
-      <c r="B517" s="3">
+      <c r="B517" s="1">
         <v>1250</v>
       </c>
       <c r="C517" s="1">
@@ -12391,8 +12408,9 @@
       <c r="E517" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F517" s="3"/>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
         <v>522</v>
       </c>
@@ -12408,8 +12426,9 @@
       <c r="E518" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F518" s="3"/>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
         <v>523</v>
       </c>
@@ -12425,8 +12444,9 @@
       <c r="E519" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F519" s="3"/>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
         <v>524</v>
       </c>
@@ -12442,8 +12462,9 @@
       <c r="E520" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F520" s="3"/>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
         <v>525</v>
       </c>
@@ -12459,8 +12480,9 @@
       <c r="E521" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F521" s="3"/>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
         <v>526</v>
       </c>
@@ -12476,8 +12498,9 @@
       <c r="E522" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F522" s="3"/>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
         <v>527</v>
       </c>
@@ -12493,8 +12516,9 @@
       <c r="E523" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F523" s="3"/>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
         <v>528</v>
       </c>
@@ -12504,14 +12528,15 @@
       <c r="C524" s="1">
         <v>238</v>
       </c>
-      <c r="D524" s="3">
+      <c r="D524" s="1">
         <v>1412</v>
       </c>
       <c r="E524" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F524" s="3"/>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
         <v>529</v>
       </c>
@@ -12527,12 +12552,13 @@
       <c r="E525" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F525" s="3"/>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
         <v>530</v>
       </c>
-      <c r="B526" s="3">
+      <c r="B526" s="1">
         <v>1223</v>
       </c>
       <c r="C526" s="1">
@@ -12544,8 +12570,9 @@
       <c r="E526" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="527" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F526" s="3"/>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
         <v>531</v>
       </c>
@@ -12555,14 +12582,15 @@
       <c r="C527" s="1">
         <v>87</v>
       </c>
-      <c r="D527" s="3">
+      <c r="D527" s="1">
         <v>2239</v>
       </c>
       <c r="E527" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="528" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F527" s="3"/>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
         <v>532</v>
       </c>
@@ -12572,31 +12600,33 @@
       <c r="C528" s="1">
         <v>163</v>
       </c>
-      <c r="D528" s="3">
+      <c r="D528" s="1">
         <v>1499</v>
       </c>
       <c r="E528" s="1">
         <v>385</v>
       </c>
-    </row>
-    <row r="529" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F528" s="3"/>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>533</v>
       </c>
-      <c r="B529" s="3">
+      <c r="B529" s="1">
         <v>2467</v>
       </c>
-      <c r="C529" s="3">
+      <c r="C529" s="1">
         <v>1119</v>
       </c>
-      <c r="D529" s="3">
+      <c r="D529" s="1">
         <v>1583</v>
       </c>
       <c r="E529" s="1">
         <v>356</v>
       </c>
-    </row>
-    <row r="530" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F529" s="3"/>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>534</v>
       </c>
@@ -12612,12 +12642,13 @@
       <c r="E530" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="531" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F530" s="3"/>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>535</v>
       </c>
-      <c r="B531" s="3">
+      <c r="B531" s="1">
         <v>1976</v>
       </c>
       <c r="C531" s="1">
@@ -12629,8 +12660,9 @@
       <c r="E531" s="1">
         <v>394</v>
       </c>
-    </row>
-    <row r="532" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F531" s="3"/>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>536</v>
       </c>
@@ -12646,25 +12678,27 @@
       <c r="E532" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="533" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F532" s="3"/>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>537</v>
       </c>
-      <c r="B533" s="3">
+      <c r="B533" s="1">
         <v>1732</v>
       </c>
-      <c r="C533" s="3">
+      <c r="C533" s="1">
         <v>1232</v>
       </c>
-      <c r="D533" s="3">
+      <c r="D533" s="1">
         <v>6344</v>
       </c>
-      <c r="E533" s="3">
+      <c r="E533" s="1">
         <v>1839</v>
       </c>
-    </row>
-    <row r="534" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F533" s="3"/>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>538</v>
       </c>
@@ -12680,8 +12714,9 @@
       <c r="E534" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="535" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F534" s="3"/>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>539</v>
       </c>
@@ -12691,14 +12726,15 @@
       <c r="C535" s="1">
         <v>129</v>
       </c>
-      <c r="D535" s="3">
+      <c r="D535" s="1">
         <v>1347</v>
       </c>
       <c r="E535" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="536" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F535" s="3"/>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>540</v>
       </c>
@@ -12714,8 +12750,9 @@
       <c r="E536" s="1">
         <v>136</v>
       </c>
-    </row>
-    <row r="537" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F536" s="3"/>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>541</v>
       </c>
@@ -12725,14 +12762,15 @@
       <c r="C537" s="1">
         <v>105</v>
       </c>
-      <c r="D537" s="3">
+      <c r="D537" s="1">
         <v>1017</v>
       </c>
       <c r="E537" s="1">
         <v>318</v>
       </c>
-    </row>
-    <row r="538" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F537" s="3"/>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>542</v>
       </c>
@@ -12748,8 +12786,9 @@
       <c r="E538" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="539" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F538" s="3"/>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>543</v>
       </c>
@@ -12759,18 +12798,19 @@
       <c r="C539" s="1">
         <v>362</v>
       </c>
-      <c r="D539" s="3">
+      <c r="D539" s="1">
         <v>1441</v>
       </c>
       <c r="E539" s="1">
         <v>351</v>
       </c>
-    </row>
-    <row r="540" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F539" s="3"/>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>544</v>
       </c>
-      <c r="B540" s="3">
+      <c r="B540" s="1">
         <v>3525</v>
       </c>
       <c r="C540" s="1">
@@ -12782,8 +12822,9 @@
       <c r="E540" s="1">
         <v>596</v>
       </c>
-    </row>
-    <row r="541" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F540" s="3"/>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>545</v>
       </c>
@@ -12799,8 +12840,9 @@
       <c r="E541" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="542" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F541" s="3"/>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>546</v>
       </c>
@@ -12816,25 +12858,27 @@
       <c r="E542" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="543" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F542" s="3"/>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>547</v>
       </c>
-      <c r="B543" s="3">
+      <c r="B543" s="1">
         <v>2506</v>
       </c>
-      <c r="C543" s="3">
+      <c r="C543" s="1">
         <v>1759</v>
       </c>
-      <c r="D543" s="3">
+      <c r="D543" s="1">
         <v>1004</v>
       </c>
-      <c r="E543" s="3">
+      <c r="E543" s="1">
         <v>1480</v>
       </c>
-    </row>
-    <row r="544" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F543" s="3"/>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>548</v>
       </c>
@@ -12844,14 +12888,15 @@
       <c r="C544" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D544" s="3">
+      <c r="D544" s="1">
         <v>1114</v>
       </c>
       <c r="E544" s="1">
         <v>262</v>
       </c>
-    </row>
-    <row r="545" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F544" s="3"/>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
         <v>549</v>
       </c>
@@ -12867,8 +12912,9 @@
       <c r="E545" s="1">
         <v>181</v>
       </c>
-    </row>
-    <row r="546" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F545" s="3"/>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
         <v>550</v>
       </c>
@@ -12884,8 +12930,9 @@
       <c r="E546" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="547" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F546" s="3"/>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
         <v>551</v>
       </c>
@@ -12895,14 +12942,15 @@
       <c r="C547" s="1">
         <v>285</v>
       </c>
-      <c r="D547" s="3">
+      <c r="D547" s="1">
         <v>1036</v>
       </c>
       <c r="E547" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="548" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F547" s="3"/>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
         <v>552</v>
       </c>
@@ -12918,8 +12966,9 @@
       <c r="E548" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="549" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F548" s="3"/>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
         <v>553</v>
       </c>
@@ -12935,8 +12984,9 @@
       <c r="E549" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="550" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F549" s="3"/>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
         <v>554</v>
       </c>
@@ -12952,8 +13002,9 @@
       <c r="E550" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="551" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F550" s="3"/>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
         <v>555</v>
       </c>
@@ -12969,8 +13020,9 @@
       <c r="E551" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="552" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F551" s="3"/>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
         <v>556</v>
       </c>
@@ -12986,8 +13038,9 @@
       <c r="E552" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="553" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F552" s="3"/>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
         <v>557</v>
       </c>
@@ -12997,14 +13050,15 @@
       <c r="C553" s="1">
         <v>402</v>
       </c>
-      <c r="D553" s="3">
+      <c r="D553" s="1">
         <v>1946</v>
       </c>
       <c r="E553" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="554" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F553" s="3"/>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>558</v>
       </c>
@@ -13020,8 +13074,9 @@
       <c r="E554" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="555" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F554" s="3"/>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
         <v>559</v>
       </c>
@@ -13037,8 +13092,9 @@
       <c r="E555" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="556" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F555" s="3"/>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
         <v>560</v>
       </c>
@@ -13054,8 +13110,9 @@
       <c r="E556" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="557" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F556" s="3"/>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
         <v>561</v>
       </c>
@@ -13071,8 +13128,9 @@
       <c r="E557" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="558" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F557" s="3"/>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
         <v>562</v>
       </c>
@@ -13082,14 +13140,15 @@
       <c r="C558" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D558" s="3">
+      <c r="D558" s="1">
         <v>1041</v>
       </c>
       <c r="E558" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="559" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F558" s="3"/>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
         <v>563</v>
       </c>
@@ -13105,8 +13164,9 @@
       <c r="E559" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="560" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F559" s="3"/>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
         <v>564</v>
       </c>
@@ -13122,8 +13182,9 @@
       <c r="E560" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="561" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F560" s="3"/>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>565</v>
       </c>
@@ -13139,8 +13200,9 @@
       <c r="E561" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="562" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F561" s="3"/>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>566</v>
       </c>
@@ -13156,8 +13218,9 @@
       <c r="E562" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="563" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F562" s="3"/>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>567</v>
       </c>
@@ -13173,8 +13236,9 @@
       <c r="E563" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="564" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F563" s="3"/>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
         <v>568</v>
       </c>
@@ -13190,8 +13254,9 @@
       <c r="E564" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="565" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F564" s="3"/>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>569</v>
       </c>
@@ -13207,8 +13272,9 @@
       <c r="E565" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="566" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F565" s="3"/>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
         <v>570</v>
       </c>
@@ -13224,8 +13290,9 @@
       <c r="E566" s="1">
         <v>57</v>
       </c>
-    </row>
-    <row r="567" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F566" s="3"/>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>571</v>
       </c>
@@ -13235,14 +13302,15 @@
       <c r="C567" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D567" s="3">
+      <c r="D567" s="1">
         <v>1272</v>
       </c>
       <c r="E567" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="568" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F567" s="3"/>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
         <v>572</v>
       </c>
@@ -13258,8 +13326,9 @@
       <c r="E568" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="569" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F568" s="3"/>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>573</v>
       </c>
@@ -13275,8 +13344,9 @@
       <c r="E569" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="570" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F569" s="3"/>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
         <v>574</v>
       </c>
@@ -13286,12 +13356,13 @@
       <c r="C570" s="2">
         <v>711</v>
       </c>
-      <c r="D570" s="4">
+      <c r="D570" s="2">
         <v>4782</v>
       </c>
       <c r="E570" s="2">
         <v>974</v>
       </c>
+      <c r="F570" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>